<commit_message>
Updated identifiers and added BOMs
</commit_message>
<xml_diff>
--- a/Electron/V2/BOM.xlsx
+++ b/Electron/V2/BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\github\ThingOnAStick\EnvironmentOnAStick\Electron\V2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\github\ThingySticks\EnvironmentMonitor\Electron\V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>U4</t>
   </si>
@@ -89,15 +89,9 @@
     <t>C1,C4</t>
   </si>
   <si>
-    <t>U$1</t>
-  </si>
-  <si>
     <t>Photon or Electron</t>
   </si>
   <si>
-    <t>Headers, 12 or 18W</t>
-  </si>
-  <si>
     <t>Environment Sensor. Version 2. Bill of Materials</t>
   </si>
   <si>
@@ -114,13 +108,58 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Reel</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>1k5</t>
+  </si>
+  <si>
+    <t>"1206"</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>Reverse LED Blue</t>
+  </si>
+  <si>
+    <t>Headers 12W</t>
+  </si>
+  <si>
+    <t>Headers 18W</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>U3a</t>
+  </si>
+  <si>
+    <t>U3b</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>Wholesale:</t>
+  </si>
+  <si>
+    <t>Retail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,6 +169,14 @@
     </font>
     <font>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -156,9 +203,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,20 +501,20 @@
     <col min="7" max="7" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
@@ -483,11 +531,17 @@
       <c r="G3" t="s">
         <v>10</v>
       </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
       <c r="I3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -500,15 +554,21 @@
       <c r="D4">
         <v>2</v>
       </c>
+      <c r="E4">
+        <v>2.9100000000000001E-2</v>
+      </c>
       <c r="F4">
         <f>E4*D4</f>
-        <v>0</v>
+        <v>5.8200000000000002E-2</v>
       </c>
       <c r="G4">
         <v>2320853</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>2310412</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -521,12 +581,21 @@
       <c r="D5">
         <v>2</v>
       </c>
+      <c r="E5">
+        <v>8.9999999999999998E-4</v>
+      </c>
       <c r="F5">
-        <f t="shared" ref="F5:F13" si="0">E5*D5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" ref="F5:F17" si="0">E5*D5</f>
+        <v>1.8E-3</v>
+      </c>
+      <c r="G5">
+        <v>9333266</v>
+      </c>
+      <c r="H5">
+        <v>2129167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -539,132 +608,267 @@
       <c r="D6">
         <v>1</v>
       </c>
+      <c r="E6">
+        <v>8.9999999999999998E-4</v>
+      </c>
       <c r="F6">
         <f t="shared" si="0"/>
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="G6">
+        <v>9332391</v>
+      </c>
+      <c r="H6">
+        <v>2129195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="G7">
+        <v>9335951</v>
+      </c>
+      <c r="H7">
+        <v>2129658</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>1206</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0.68</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0.68</v>
+      </c>
+      <c r="G8">
+        <v>1497671</v>
+      </c>
+      <c r="J8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>2.5</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G9">
+        <v>2393536</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>2.63</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>2.63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0.106</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0.106</v>
+      </c>
+      <c r="G11">
+        <v>9555986</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0.23</v>
+      </c>
+      <c r="F12">
+        <f>E12*D12</f>
+        <v>0.23</v>
+      </c>
+      <c r="G12">
+        <v>2217907</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0.35</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0.35</v>
+      </c>
+      <c r="G13">
+        <v>2476092</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>1206</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>0.96</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="0"/>
-        <v>0.96</v>
-      </c>
-      <c r="G7">
-        <v>1497671</v>
-      </c>
-      <c r="I7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>3.07</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>3.07</v>
-      </c>
-      <c r="G8">
-        <v>2393536</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
+      <c r="E15">
+        <v>9.11E-2</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0.1822</v>
+      </c>
+      <c r="G15">
+        <v>1593465</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="F10">
+      <c r="F16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G10">
-        <v>9555986</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>0</v>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1.5</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="2">
+        <f>SUM(F4:F17)</f>
+        <v>8.2403999999999993</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20">
+        <f>F18*2</f>
+        <v>16.480799999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21">
+        <f>F20*2</f>
+        <v>32.961599999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>